<commit_message>
Export list transactions of general ledger
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/excel/Template_E_GeneralLedger.xlsx
+++ b/src/main/resources/static/templates/excel/Template_E_GeneralLedger.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App\FW_PMS\src\main\resources\static\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7527A6BE-246D-4DCF-961F-7AB102599623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C66DF5C-0B17-4634-A596-353E947D58C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Danh sách sản phẩm" sheetId="1" r:id="rId1"/>
+    <sheet name="Sổ quỹ" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,45 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FLOWIEE OFFICIAL</t>
   </si>
   <si>
-    <t>Danh sách sản phẩm</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Loại sản phẩm</t>
-  </si>
-  <si>
-    <t>Tên sản phẩm</t>
-  </si>
-  <si>
-    <t>Kích cỡ</t>
-  </si>
-  <si>
-    <t>Màu sắc</t>
-  </si>
-  <si>
-    <t>Số lượng</t>
-  </si>
-  <si>
-    <t>Đã bán</t>
-  </si>
-  <si>
-    <t>Giá khuyến mãi</t>
-  </si>
-  <si>
-    <t>Giá gốc</t>
-  </si>
-  <si>
-    <t>Chất liệu</t>
-  </si>
-  <si>
-    <t>Trạng thái</t>
+    <t>Mã phiếu</t>
+  </si>
+  <si>
+    <t>Loại phiếu</t>
+  </si>
+  <si>
+    <t>Giá trị</t>
+  </si>
+  <si>
+    <t>Ngày tạo</t>
+  </si>
+  <si>
+    <t>Mã chứng từ</t>
+  </si>
+  <si>
+    <t>Người tạo</t>
+  </si>
+  <si>
+    <t>Người nộp/ nhận</t>
+  </si>
+  <si>
+    <t>Nội dung</t>
+  </si>
+  <si>
+    <t>Sổ quỹ</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
   </si>
 </sst>
 </file>
@@ -158,21 +155,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,26 +557,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMI19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="1023" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -588,12 +587,10 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -603,256 +600,219 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>